<commit_message>
Added Photo to Excel database.  Migrated legacy photo data to Excel import schema.
git-svn-id: https://subversion.assembla.com/svn/treesdb/branches/ExcelImport@314 d913c9e1-59cf-094f-9d4b-ab1779aea92f
</commit_message>
<xml_diff>
--- a/TMD/_TMD.xlsx
+++ b/TMD/_TMD.xlsx
@@ -3,6 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="14505" yWindow="-15" windowWidth="14310" windowHeight="14355" tabRatio="408"/>
   </bookViews>
@@ -12,6 +13,7 @@
     <sheet name="Trees" sheetId="3" r:id="rId3"/>
     <sheet name="Trunks" sheetId="4" r:id="rId4"/>
     <sheet name="Internal" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="Photos" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Trees!$B$3:$B$100003</definedName>
@@ -19,6 +21,7 @@
     <definedName name="ClinometerBrands">Internal!$Q$2:$Q$5</definedName>
     <definedName name="CrownSpreadMeasurementMethods">Internal!$M$2:$M$3</definedName>
     <definedName name="CrownVolumeCalculationMethods">Internal!$N$2:$N$3</definedName>
+    <definedName name="E">Photos!$C$2</definedName>
     <definedName name="_xlnm.Extract" localSheetId="2">Trees!#REF!</definedName>
     <definedName name="HeightMeasurementMethods">Internal!$D$2:$D$9</definedName>
     <definedName name="HeightMeasurementTypes">Internal!$E$2:$E$4</definedName>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3982" uniqueCount="3592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="3597">
   <si>
     <t>Latitude</t>
   </si>
@@ -10930,16 +10933,51 @@
   <si>
     <t>Terrain</t>
   </si>
+  <si>
+    <t>Site Name</t>
+  </si>
+  <si>
+    <t>Subsite Name</t>
+  </si>
+  <si>
+    <r>
+      <t>Filename</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Caption</t>
+  </si>
+  <si>
+    <t>Photographer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -11043,6 +11081,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -11070,7 +11116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -11179,15 +11225,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -11198,116 +11235,133 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="30">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
@@ -11803,7 +11857,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="11.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="5" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.42578125" style="5" customWidth="1"/>
@@ -11861,9 +11916,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="E1:E1048576">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" sqref="A1:A1048576">
-      <formula1>COUNTIF(A:A, A1)&lt;=1</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="A1:A1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" sqref="D1:D1048576 F1:F1048576 G1:G1048576"/>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -11894,8 +11947,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.140625" style="5" customWidth="1"/>
     <col min="3" max="8" width="11.42578125" style="5" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.140625" style="5" bestFit="1" customWidth="1"/>
@@ -11953,15 +12005,13 @@
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Example" prompt="-80.12345" sqref="G1:G1048576"/>
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Example" prompt="40.12345" sqref="F1:F1048576"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Explanation" prompt="Associate this Subsite to a Site" sqref="A1:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="Explanation" prompt="Associate this Subsite with a Site" sqref="A1:A1048576">
       <formula1>SiteNames</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="I1:I1048576">
       <formula1>SiteOwnershipTypes</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" sqref="B1:B1048576">
-      <formula1>COUNTIF(B:B, B1)&lt;=1</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="B1:B1048576"/>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -11983,7 +12033,7 @@
   <dimension ref="A1:BA12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
@@ -11991,8 +12041,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="5" customWidth="1"/>
+    <col min="1" max="2" width="22.140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="16" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="5" customWidth="1"/>
@@ -12044,145 +12093,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="26" t="s">
         <v>3567</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="28" t="s">
         <v>3566</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="30" t="s">
         <v>3525</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="31" t="s">
         <v>3526</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="16" t="s">
         <v>3585</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="21" t="s">
         <v>3572</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="16" t="s">
         <v>3569</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="22" t="s">
         <v>3523</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="22" t="s">
         <v>3524</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="17" t="s">
         <v>3543</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="T1" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="U1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="V1" s="32" t="s">
+      <c r="V1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="W1" s="20" t="s">
         <v>3582</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="X1" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="Y1" s="25" t="s">
+      <c r="Y1" s="16" t="s">
         <v>3588</v>
       </c>
-      <c r="Z1" s="16" t="s">
+      <c r="Z1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="16" t="s">
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="16" t="s">
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="24" t="s">
         <v>3589</v>
       </c>
-      <c r="AM1" s="16"/>
-      <c r="AN1" s="16"/>
-      <c r="AO1" s="16"/>
-      <c r="AP1" s="16"/>
-      <c r="AQ1" s="16"/>
-      <c r="AR1" s="16"/>
-      <c r="AS1" s="17"/>
-      <c r="AT1" s="15" t="s">
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="23" t="s">
         <v>3590</v>
       </c>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="16"/>
-      <c r="AW1" s="16"/>
-      <c r="AX1" s="15" t="s">
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="23" t="s">
         <v>3591</v>
       </c>
-      <c r="AY1" s="16"/>
-      <c r="AZ1" s="17"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="25"/>
     </row>
     <row r="2" spans="1:52" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="25"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="16"/>
       <c r="Z2" s="4" t="s">
         <v>124</v>
       </c>
@@ -12269,20 +12318,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0" insertHyperlinks="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="30">
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="Y1:Y2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="AX1:AZ1"/>
     <mergeCell ref="AT1:AW1"/>
     <mergeCell ref="A1:A2"/>
@@ -12299,6 +12334,20 @@
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="U1:U2"/>
   </mergeCells>
   <dataValidations xWindow="1791" yWindow="233" count="37">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Example" prompt="345" sqref="AT1:AT1048576"/>
@@ -12399,7 +12448,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
@@ -27874,4 +27924,61 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="22.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>3592</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>3593</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3594</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>3596</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>3595</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0" insertHyperlinks="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Explanation" prompt="Associate this Photo with a Site" sqref="A1:A1048576">
+      <formula1>SiteNames</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Explanation" prompt="Associate this Photo with a Subsite" sqref="B1:B1048576">
+      <formula1>SubsiteNames</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Explanation" prompt="Associate this Photo with a Tree" sqref="C1:C1048576">
+      <formula1>TreeNames</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>